<commit_message>
- display diffs as tableview
</commit_message>
<xml_diff>
--- a/resources/TestAccount1.xlsx
+++ b/resources/TestAccount1.xlsx
@@ -7,9 +7,10 @@
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Trang tính1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
   <si>
     <t>Facebook</t>
   </si>
@@ -44,7 +45,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -58,6 +59,18 @@
       <sz val="11"/>
       <color rgb="FF4B4F56"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -89,8 +102,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -102,7 +117,9 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -435,7 +452,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -484,4 +501,61 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="47.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="13">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="13">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix bug compare two objects
</commit_message>
<xml_diff>
--- a/resources/TestAccount1.xlsx
+++ b/resources/TestAccount1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="-28420" yWindow="3560" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>Facebook</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>znpmdrz_goldmanberg_1473307997@tfbnw.net</t>
+  </si>
+  <si>
+    <t>PlaceHolder</t>
   </si>
 </sst>
 </file>
@@ -102,8 +105,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -117,9 +122,11 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -449,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -460,7 +467,7 @@
     <col min="2" max="2" width="47.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -470,8 +477,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="13">
+    <row r="2" spans="1:4" ht="13">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -481,8 +491,11 @@
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" ht="13">
+    <row r="3" spans="1:4" ht="13">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -491,10 +504,14 @@
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
add command history view and control
</commit_message>
<xml_diff>
--- a/resources/TestAccount1.xlsx
+++ b/resources/TestAccount1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Facebook</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>znpmdrz_goldmanberg_1473307997@tfbnw.net</t>
-  </si>
-  <si>
-    <t>PlaceHolder</t>
   </si>
 </sst>
 </file>
@@ -105,8 +102,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -122,11 +125,17 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -456,57 +465,207 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:A39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="2" max="2" width="47.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="13">
+    </row>
+    <row r="2" spans="1:1" ht="12">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="13">
+    </row>
+    <row r="3" spans="1:1" ht="12">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
+    </row>
+    <row r="7" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A39" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>